<commit_message>
Update chi nhánh quận 3
</commit_message>
<xml_diff>
--- a/chi phi.xlsx
+++ b/chi phi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="484" documentId="8_{BDBBFA69-30A8-4CF6-9B93-C0565901251C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AF9A11-04F3-4543-BA8B-62F00AA826A5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="4" xr2:uid="{7F4EA05D-3250-4218-93AC-E531C394224D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="3" xr2:uid="{7F4EA05D-3250-4218-93AC-E531C394224D}"/>
   </bookViews>
   <sheets>
     <sheet name="Thiết bị" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +564,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -572,9 +575,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -587,7 +587,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -905,7 +905,7 @@
       <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -917,7 +917,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -928,10 +928,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -941,7 +941,7 @@
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -978,7 +978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -995,7 +995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1055,11 +1055,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00903B39-09E6-473D-9F02-C9D91F3CF6FC}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1070,7 +1070,7 @@
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>34</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>37</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>41</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>45</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>50</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>55</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>57</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>67</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>70</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>73</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>75</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>77</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>80</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>83</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>87</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>90</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>93</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>95</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>98</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>101</v>
       </c>
@@ -1499,11 +1499,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3B5178-4682-4B89-9F44-FD05366093FE}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="132.28515625" style="4" customWidth="1"/>
@@ -1514,7 +1514,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1537,8 +1537,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1556,12 +1556,12 @@
       <c r="F2" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
       <c r="B3" s="6" t="s">
         <v>113</v>
       </c>
@@ -1573,10 +1573,10 @@
         <v>99</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="8"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="6" t="s">
         <v>114</v>
       </c>
@@ -1588,10 +1588,10 @@
         <v>115</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="8"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="6" t="s">
         <v>116</v>
       </c>
@@ -1603,10 +1603,10 @@
         <v>52</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="8"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="6" t="s">
         <v>117</v>
       </c>
@@ -1618,10 +1618,10 @@
         <v>64</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>118</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1639,12 +1639,12 @@
       <c r="F7" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="6" t="s">
         <v>124</v>
       </c>
@@ -1656,10 +1656,10 @@
         <v>126</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="6" t="s">
         <v>127</v>
       </c>
@@ -1671,10 +1671,10 @@
         <v>128</v>
       </c>
       <c r="F9" s="13"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
       <c r="B10" s="6" t="s">
         <v>129</v>
       </c>
@@ -1686,10 +1686,10 @@
         <v>130</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="30.75">
-      <c r="A11" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
       <c r="B11" s="6" t="s">
         <v>131</v>
       </c>
@@ -1701,14 +1701,14 @@
         <v>133</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="C13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>

</xml_diff>